<commit_message>
Add results for quotes to summary spreadsheet.
</commit_message>
<xml_diff>
--- a/results_summary.xlsx
+++ b/results_summary.xlsx
@@ -5,19 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="569" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="5" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="569" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="MaxEnt" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Naive Bayes" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="summary" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="movie reviews MaxEnt" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="movie reviews Naive Bayes" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="movie reviews summary" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="quotes MaxEnt" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="quotes Naive Bayes" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="quotes summary" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="45">
   <si>
     <t>features:</t>
   </si>
@@ -147,6 +150,12 @@
   <si>
     <t>Naive Bayes</t>
   </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
 </sst>
 </file>
 
@@ -228,7 +237,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -261,6 +270,10 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -281,7 +294,7 @@
   <dimension ref="A1:W62"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="I1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="Q13" activeCellId="1" pane="topLeft" sqref="K10:K11 Q13"/>
+      <selection activeCell="Q13" activeCellId="0" pane="topLeft" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2956,7 +2969,7 @@
   <dimension ref="A1:W62"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="J1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="Q13" activeCellId="1" pane="topLeft" sqref="K10:K11 Q13"/>
+      <selection activeCell="Q13" activeCellId="0" pane="topLeft" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5628,8 +5641,8 @@
   </sheetPr>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K11" activeCellId="0" pane="topLeft" sqref="K10:K11"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="K11" activeCellId="0" pane="topLeft" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -6394,4 +6407,3603 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:W30"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="R1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A13" activeCellId="0" pane="topLeft" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="16" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="79.85" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>0.476191</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>0.52381</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.654762</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>0.52381</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>0.457831</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>0.493976</v>
+      </c>
+      <c r="V8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>0.566265</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0.654762</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>0.590362</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>0.590362</v>
+      </c>
+      <c r="V9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>0.578313</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.52381</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>0.578313</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>0.542169</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>0.506024</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>0.654762</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>0.626506</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <v>0.590362</v>
+      </c>
+      <c r="V11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>0.554217</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>0.60241</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>0.518072</v>
+      </c>
+      <c r="V12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>0.542169</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <f aca="false">SUM(B3:B12)/10</f>
+        <v>0.6369048</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <f aca="false">SUM(E3:E12)/10</f>
+        <v>0.6190476</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <f aca="false">SUM(H3:H12)/10</f>
+        <v>0.6095238</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <f aca="false">SUM(K3:K12)/10</f>
+        <v>0.6000001</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <f aca="false">SUM(N3:N12)/10</f>
+        <v>0.6107142</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <f aca="false">SUM(Q3:Q12)/10</f>
+        <v>0.5641136</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T13" s="2" t="n">
+        <f aca="false">SUM(T3:T12)/10</f>
+        <v>0.5377798</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W13" s="2" t="n">
+        <f aca="false">SUM(W3:W12)/10</f>
+        <v>0.5556512</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">MIN(B3:B12)</f>
+        <v>0.535714</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">MIN(E3:E12)</f>
+        <v>0.52381</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">MIN(H3:H12)</f>
+        <v>0.535714</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">MIN(K3:K12)</f>
+        <v>0.559524</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">MIN(N3:N12)</f>
+        <v>0.535714</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <f aca="false">MIN(Q3:Q12)</f>
+        <v>0.457831</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <f aca="false">MIN(T3:T12)</f>
+        <v>0.493976</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <f aca="false">MIN(W3:W12)</f>
+        <v>0.476191</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">MAX(B3:B12)</f>
+        <v>0.678571</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">MAX(E3:E12)</f>
+        <v>0.702381</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">MAX(H3:H12)</f>
+        <v>0.654762</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">MAX(K3:K12)</f>
+        <v>0.642857</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">MAX(N3:N12)</f>
+        <v>0.690476</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <f aca="false">MAX(Q3:Q12)</f>
+        <v>0.626506</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <f aca="false">MAX(T3:T12)</f>
+        <v>0.590362</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <f aca="false">MAX(W3:W12)</f>
+        <v>0.630952</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+      <c r="A18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0.714286</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="V18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="S19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+      <c r="V19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="A20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="S20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="V20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <v>0.511905</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+      <c r="A21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="S21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="V21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+      <c r="A22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0.654762</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="S22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T22" s="0" t="n">
+        <v>0.52381</v>
+      </c>
+      <c r="V22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="W22" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="A23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0.726191</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.726191</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0.738095</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0.714286</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="S23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="T23" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+      <c r="V23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="W23" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="A24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="S24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="T24" s="0" t="n">
+        <v>0.404762</v>
+      </c>
+      <c r="V24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="W24" s="0" t="n">
+        <v>0.547619</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+      <c r="A25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="S25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="T25" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="W25" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="A26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0.654762</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>0.626506</v>
+      </c>
+      <c r="S26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T26" s="0" t="n">
+        <v>0.540121</v>
+      </c>
+      <c r="V26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="W26" s="0" t="n">
+        <v>0.530121</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="A27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="S27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="T27" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="V27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="W27" s="0" t="n">
+        <v>0.511905</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <f aca="false">SUM(B18:B27)/10</f>
+        <v>0.6488095</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <f aca="false">SUM('quotes Naive Bayes'!B18:B27)/10</f>
+        <v>0.6738096</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <f aca="false">SUM(H18:H27)/10</f>
+        <v>0.6547618</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <f aca="false">SUM(K18:K27)/10</f>
+        <v>0.6369048</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N28" s="2" t="n">
+        <f aca="false">SUM(N18:N27)/10</f>
+        <v>0.6142857</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q28" s="2" t="n">
+        <f aca="false">SUM(Q18:Q27)/10</f>
+        <v>0.6019364</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T28" s="2" t="n">
+        <f aca="false">SUM(T18:T27)/10</f>
+        <v>0.5313931</v>
+      </c>
+      <c r="V28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W28" s="2" t="n">
+        <f aca="false">SUM(W18:W27)/10</f>
+        <v>0.5565836</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">MIN(B18:B27)</f>
+        <v>0.583333</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">MIN('quotes Naive Bayes'!B18:B27)</f>
+        <v>0.607143</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">MIN(H18:H27)</f>
+        <v>0.583333</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <f aca="false">MIN(K18:K27)</f>
+        <v>0.559524</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <f aca="false">MIN(N18:N27)</f>
+        <v>0.583333</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q29" s="0" t="n">
+        <f aca="false">MIN(Q18:Q27)</f>
+        <v>0.547619</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T29" s="0" t="n">
+        <f aca="false">MIN(T18:T27)</f>
+        <v>0.404762</v>
+      </c>
+      <c r="V29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W29" s="0" t="n">
+        <f aca="false">MIN(W18:W27)</f>
+        <v>0.511905</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="A30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">MAX(B18:B27)</f>
+        <v>0.726191</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">MAX('quotes Naive Bayes'!B18:B27)</f>
+        <v>0.75</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">MAX(H18:H27)</f>
+        <v>0.738095</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <f aca="false">MAX(K18:K27)</f>
+        <v>0.714286</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <f aca="false">MAX(N18:N27)</f>
+        <v>0.690476</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q30" s="0" t="n">
+        <f aca="false">MAX(Q18:Q27)</f>
+        <v>0.678571</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T30" s="0" t="n">
+        <f aca="false">MAX(T18:T27)</f>
+        <v>0.583333</v>
+      </c>
+      <c r="V30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W30" s="0" t="n">
+        <f aca="false">MAX(W18:W27)</f>
+        <v>0.607143</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:W30"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="P1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A13" activeCellId="0" pane="topLeft" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="16" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="79.85" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0.476191</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <v>0.464286</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>0.428571</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.52381</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>0.511905</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>0.488095</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.714286</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.738095</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.726191</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>0.52381</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>0.511905</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.785714</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0.726191</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>0.530121</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>0.518072</v>
+      </c>
+      <c r="V8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>0.554217</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>0.614458</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>0.493976</v>
+      </c>
+      <c r="V9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>0.554217</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>0.542169</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>0.493976</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>0.46988</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>0.638554</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <v>0.493976</v>
+      </c>
+      <c r="V11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>0.506024</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="8" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>0.650602</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>0.433735</v>
+      </c>
+      <c r="V12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>0.481928</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <f aca="false">SUM(B3:B12)/10</f>
+        <v>0.6452381</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <f aca="false">SUM(E3:E12)/10</f>
+        <v>0.6559523</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <f aca="false">SUM(H3:H12)/10</f>
+        <v>0.6380951</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <f aca="false">SUM(K3:K12)/10</f>
+        <v>0.6214286</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <f aca="false">SUM(N3:N12)/10</f>
+        <v>0.6071426</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="2" t="n">
+        <f aca="false">SUM(Q3:Q12)/10</f>
+        <v>0.5999713</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T13" s="2" t="n">
+        <f aca="false">SUM(T3:T12)/10</f>
+        <v>0.499326</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W13" s="2" t="n">
+        <f aca="false">SUM(W3:W12)/10</f>
+        <v>0.5137694</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">MIN(B3:B12)</f>
+        <v>0.583333</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">MIN(E3:E12)</f>
+        <v>0.583333</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">MIN(H3:H12)</f>
+        <v>0.535714</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">MIN(K3:K12)</f>
+        <v>0.52381</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">MIN(N3:N12)</f>
+        <v>0.535714</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <f aca="false">MIN(Q3:Q12)</f>
+        <v>0.476191</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <f aca="false">MIN(T3:T12)</f>
+        <v>0.433735</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <f aca="false">MIN(W3:W12)</f>
+        <v>0.428571</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">MAX(B3:B12)</f>
+        <v>0.714286</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">MAX(E3:E12)</f>
+        <v>0.785714</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">MAX(H3:H12)</f>
+        <v>0.726191</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">MAX(K3:K12)</f>
+        <v>0.726191</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">MAX(N3:N12)</f>
+        <v>0.690476</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <f aca="false">MAX(Q3:Q12)</f>
+        <v>0.678571</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <f aca="false">MAX(T3:T12)</f>
+        <v>0.559524</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <f aca="false">MAX(W3:W12)</f>
+        <v>0.607143</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+      <c r="A17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+      <c r="A18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0.654762</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0.738095</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>0.654762</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.726191</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0.738095</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="S19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="V19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <v>0.511905</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="A20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="S20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="V20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <v>0.547619</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+      <c r="A21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.726191</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0.654762</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="S21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="V21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+      <c r="A22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="S22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T22" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="W22" s="0" t="n">
+        <v>0.559524</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="A23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0.77381</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0.654762</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="S23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="T23" s="0" t="n">
+        <v>0.619048</v>
+      </c>
+      <c r="V23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="W23" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="A24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="S24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="T24" s="0" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="V24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="W24" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+      <c r="A25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0.630952</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+      <c r="S25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="T25" s="0" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="V25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="W25" s="0" t="n">
+        <v>0.571429</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="A26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>0.650602</v>
+      </c>
+      <c r="S26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T26" s="0" t="n">
+        <v>0.518072</v>
+      </c>
+      <c r="V26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="W26" s="0" t="n">
+        <v>0.578313</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="A27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="S27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="T27" s="0" t="n">
+        <v>0.464286</v>
+      </c>
+      <c r="V27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="W27" s="0" t="n">
+        <v>0.535714</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <f aca="false">SUM(B18:B27)/10</f>
+        <v>0.6738096</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <f aca="false">SUM(E18:E27)/10</f>
+        <v>0.6202381</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <f aca="false">SUM(H18:H27)/10</f>
+        <v>0.6833334</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <f aca="false">SUM(K18:K27)/10</f>
+        <v>0.5952379</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N28" s="2" t="n">
+        <f aca="false">SUM(N18:N27)/10</f>
+        <v>0.6130953</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q28" s="2" t="n">
+        <f aca="false">SUM(Q18:Q27)/10</f>
+        <v>0.6174411</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T28" s="2" t="n">
+        <f aca="false">SUM(T18:T27)/10</f>
+        <v>0.5565692</v>
+      </c>
+      <c r="V28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W28" s="2" t="n">
+        <f aca="false">SUM(W18:W27)/10</f>
+        <v>0.5590219</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="A29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">MIN(B18:B27)</f>
+        <v>0.607143</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">MIN(E18:E27)</f>
+        <v>0.571429</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">MIN(H18:H27)</f>
+        <v>0.595238</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <f aca="false">MIN(K18:K27)</f>
+        <v>0.535714</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <f aca="false">MIN(N18:N27)</f>
+        <v>0.535714</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q29" s="0" t="n">
+        <f aca="false">MIN(Q18:Q27)</f>
+        <v>0.535714</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T29" s="0" t="n">
+        <f aca="false">MIN(T18:T27)</f>
+        <v>0.464286</v>
+      </c>
+      <c r="V29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W29" s="0" t="n">
+        <f aca="false">MIN(W18:W27)</f>
+        <v>0.511905</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="A30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">MAX(B18:B27)</f>
+        <v>0.75</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">MAX(E18:E27)</f>
+        <v>0.702381</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">MAX(H18:H27)</f>
+        <v>0.77381</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <f aca="false">MAX(K18:K27)</f>
+        <v>0.654762</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <f aca="false">MAX(N18:N27)</f>
+        <v>0.666667</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q30" s="0" t="n">
+        <f aca="false">MAX(Q18:Q27)</f>
+        <v>0.702381</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T30" s="0" t="n">
+        <f aca="false">MAX(T18:T27)</f>
+        <v>0.642857</v>
+      </c>
+      <c r="V30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W30" s="0" t="n">
+        <f aca="false">MAX(W18:W27)</f>
+        <v>0.607143</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="H41" activeCellId="0" pane="topLeft" sqref="H41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.1"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>0.6488095</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>0.726191</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>0.6369048</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0.678571</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="B5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>0.6738096</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>0.6190476</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>0.52381</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0.702381</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+      <c r="A6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>0.6547618</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>0.738095</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <v>0.6095238</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0.654762</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="B7" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>0.6369048</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>0.714286</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>0.6000001</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0.642857</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="B8" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>0.6142857</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>0.6107142</v>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0.690476</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>0.6019364</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="F9" s="7" t="n">
+        <v>0.5641136</v>
+      </c>
+      <c r="G9" s="7" t="n">
+        <v>0.457831</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0.626506</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="B10" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>0.5313931</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>0.404762</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>0.5377798</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>0.493976</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0.590362</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="B11" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>0.5565836</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>0.511905</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <v>0.5556512</v>
+      </c>
+      <c r="G11" s="7" t="n">
+        <v>0.476191</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0.630952</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
+      <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="A16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
+      <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7" t="n">
+        <v>0.6738096</v>
+      </c>
+      <c r="D17" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="E17" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F17" s="7" t="n">
+        <v>0.6452381</v>
+      </c>
+      <c r="G17" s="7" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>0.714286</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+      <c r="B18" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" s="7" t="n">
+        <v>0.6202381</v>
+      </c>
+      <c r="D18" s="7" t="n">
+        <v>0.571429</v>
+      </c>
+      <c r="E18" s="7" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="F18" s="7" t="n">
+        <v>0.6559523</v>
+      </c>
+      <c r="G18" s="7" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <v>0.785714</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
+      <c r="A19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7" t="n">
+        <v>0.6833334</v>
+      </c>
+      <c r="D19" s="7" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="E19" s="7" t="n">
+        <v>0.77381</v>
+      </c>
+      <c r="F19" s="7" t="n">
+        <v>0.6380951</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="H19" s="7" t="n">
+        <v>0.726191</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="B20" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="7" t="n">
+        <v>0.5952379</v>
+      </c>
+      <c r="D20" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="E20" s="7" t="n">
+        <v>0.654762</v>
+      </c>
+      <c r="F20" s="7" t="n">
+        <v>0.6214286</v>
+      </c>
+      <c r="G20" s="7" t="n">
+        <v>0.52381</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <v>0.726191</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+      <c r="B21" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="7" t="n">
+        <v>0.6130953</v>
+      </c>
+      <c r="D21" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="E21" s="7" t="n">
+        <v>0.666667</v>
+      </c>
+      <c r="F21" s="7" t="n">
+        <v>0.6071426</v>
+      </c>
+      <c r="G21" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="H21" s="7" t="n">
+        <v>0.690476</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+      <c r="A22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7" t="n">
+        <v>0.6174411</v>
+      </c>
+      <c r="D22" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="E22" s="7" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="F22" s="7" t="n">
+        <v>0.5999713</v>
+      </c>
+      <c r="G22" s="7" t="n">
+        <v>0.476191</v>
+      </c>
+      <c r="H22" s="7" t="n">
+        <v>0.678571</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="B23" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="7" t="n">
+        <v>0.5565692</v>
+      </c>
+      <c r="D23" s="7" t="n">
+        <v>0.464286</v>
+      </c>
+      <c r="E23" s="7" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="F23" s="7" t="n">
+        <v>0.499326</v>
+      </c>
+      <c r="G23" s="7" t="n">
+        <v>0.433735</v>
+      </c>
+      <c r="H23" s="7" t="n">
+        <v>0.559524</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="B24" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="7" t="n">
+        <v>0.5590219</v>
+      </c>
+      <c r="D24" s="7" t="n">
+        <v>0.511905</v>
+      </c>
+      <c r="E24" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="F24" s="7" t="n">
+        <v>0.5137694</v>
+      </c>
+      <c r="G24" s="7" t="n">
+        <v>0.428571</v>
+      </c>
+      <c r="H24" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update results spreadsheet with negation tagged results.
</commit_message>
<xml_diff>
--- a/results_summary.xlsx
+++ b/results_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="569" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="809" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="movie reviews MaxEnt" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="48">
   <si>
     <t>features:</t>
   </si>
@@ -130,10 +130,16 @@
     <t>cut-off</t>
   </si>
   <si>
+    <t>negation</t>
+  </si>
+  <si>
     <t>unigram</t>
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t>bigram</t>
@@ -146,6 +152,9 @@
   </si>
   <si>
     <t>sentiment lexicon</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t>Naive Bayes</t>
@@ -237,7 +246,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -267,6 +276,10 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -5639,17 +5652,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K11" activeCellId="0" pane="topLeft" sqref="K11"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="H39" activeCellId="0" pane="topLeft" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.1"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -5663,22 +5676,24 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4"/>
       <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="4" t="s">
@@ -5687,48 +5702,54 @@
       <c r="B3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="7" t="n">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="7" t="n">
         <v>0.86</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="E4" s="7" t="n">
         <v>0.81</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="F4" s="7" t="n">
         <v>0.915</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="G4" s="7" t="n">
         <v>0.834</v>
       </c>
-      <c r="G4" s="7" t="n">
+      <c r="H4" s="7" t="n">
         <v>0.815</v>
       </c>
-      <c r="H4" s="7" t="n">
+      <c r="I4" s="7" t="n">
         <v>0.86</v>
       </c>
     </row>
@@ -5736,22 +5757,25 @@
       <c r="B5" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="7" t="n">
         <v>0.863</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="E5" s="7" t="n">
         <v>0.815</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="F5" s="7" t="n">
         <v>0.915</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="G5" s="7" t="n">
         <v>0.838</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="H5" s="7" t="n">
         <v>0.805</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="I5" s="7" t="n">
         <v>0.88</v>
       </c>
     </row>
@@ -5759,48 +5783,54 @@
       <c r="B6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="7" t="n">
         <v>0.8605</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="E6" s="7" t="n">
         <v>0.82</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="F6" s="7" t="n">
         <v>0.9</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="G6" s="7" t="n">
         <v>0.8285</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="H6" s="7" t="n">
         <v>0.75</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="I6" s="7" t="n">
         <v>0.845</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
       <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="7" t="n">
         <v>0.8465</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="E7" s="7" t="n">
         <v>0.805</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="F7" s="7" t="n">
         <v>0.88</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="G7" s="7" t="n">
         <v>0.831</v>
       </c>
-      <c r="G7" s="7" t="n">
+      <c r="H7" s="7" t="n">
         <v>0.78</v>
       </c>
-      <c r="H7" s="7" t="n">
+      <c r="I7" s="7" t="n">
         <v>0.87</v>
       </c>
     </row>
@@ -5808,22 +5838,25 @@
       <c r="B8" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="7" t="n">
         <v>0.835</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="E8" s="7" t="n">
         <v>0.81</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="F8" s="7" t="n">
         <v>0.86</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="G8" s="7" t="n">
         <v>0.809</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="H8" s="7" t="n">
         <v>0.75</v>
       </c>
-      <c r="H8" s="7" t="n">
+      <c r="I8" s="7" t="n">
         <v>0.845</v>
       </c>
     </row>
@@ -5831,22 +5864,25 @@
       <c r="B9" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="7" t="n">
         <v>0.815</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="E9" s="7" t="n">
         <v>0.78</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="F9" s="7" t="n">
         <v>0.85</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="G9" s="7" t="n">
         <v>0.797</v>
       </c>
-      <c r="G9" s="7" t="n">
+      <c r="H9" s="7" t="n">
         <v>0.74</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="I9" s="7" t="n">
         <v>0.855</v>
       </c>
     </row>
@@ -5854,48 +5890,54 @@
       <c r="B10" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="7" t="n">
         <v>0.8115</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="E10" s="7" t="n">
         <v>0.785</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="F10" s="7" t="n">
         <v>0.86</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="G10" s="7" t="n">
         <v>0.793</v>
       </c>
-      <c r="G10" s="7" t="n">
+      <c r="H10" s="7" t="n">
         <v>0.74</v>
       </c>
-      <c r="H10" s="7" t="n">
+      <c r="I10" s="7" t="n">
         <v>0.845</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="7" t="n">
+      <c r="D11" s="7" t="n">
         <v>0.5005</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="E11" s="7" t="n">
         <v>0.495</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="F11" s="7" t="n">
         <v>0.51</v>
       </c>
-      <c r="F11" s="7" t="n">
+      <c r="G11" s="7" t="n">
         <v>0.818</v>
       </c>
-      <c r="G11" s="7" t="n">
+      <c r="H11" s="7" t="n">
         <v>0.76</v>
       </c>
-      <c r="H11" s="7" t="n">
+      <c r="I11" s="7" t="n">
         <v>0.87</v>
       </c>
     </row>
@@ -5903,22 +5945,25 @@
       <c r="B12" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="7" t="n">
         <v>0.504</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="E12" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="E12" s="7" t="n">
+      <c r="F12" s="7" t="n">
         <v>0.525</v>
       </c>
-      <c r="F12" s="7" t="n">
+      <c r="G12" s="7" t="n">
         <v>0.7855</v>
       </c>
-      <c r="G12" s="7" t="n">
+      <c r="H12" s="7" t="n">
         <v>0.725</v>
       </c>
-      <c r="H12" s="7" t="n">
+      <c r="I12" s="7" t="n">
         <v>0.83</v>
       </c>
     </row>
@@ -5926,22 +5971,25 @@
       <c r="B13" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="7" t="n">
         <v>0.7795</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="E13" s="7" t="n">
         <v>0.725</v>
       </c>
-      <c r="E13" s="7" t="n">
+      <c r="F13" s="7" t="n">
         <v>0.81</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="G13" s="7" t="n">
         <v>0.768</v>
       </c>
-      <c r="G13" s="7" t="n">
+      <c r="H13" s="7" t="n">
         <v>0.725</v>
       </c>
-      <c r="H13" s="7" t="n">
+      <c r="I13" s="7" t="n">
         <v>0.82</v>
       </c>
     </row>
@@ -5949,455 +5997,981 @@
       <c r="B14" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="7" t="n">
         <v>0.762</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="E14" s="7" t="n">
         <v>0.72</v>
       </c>
-      <c r="E14" s="7" t="n">
+      <c r="F14" s="7" t="n">
         <v>0.79</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="G14" s="7" t="n">
         <v>0.75655</v>
       </c>
-      <c r="G14" s="7" t="n">
+      <c r="H14" s="7" t="n">
         <v>0.7</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="I14" s="7" t="n">
         <v>0.7955</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
       <c r="A15" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="7" t="n">
+        <v>38</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="7" t="n">
         <v>0.8535</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="E15" s="7" t="n">
         <v>0.825</v>
       </c>
-      <c r="E15" s="7" t="n">
+      <c r="F15" s="7" t="n">
         <v>0.89</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="G15" s="7" t="n">
         <v>0.827</v>
       </c>
-      <c r="G15" s="7" t="n">
+      <c r="H15" s="7" t="n">
         <v>0.795</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="I15" s="7" t="n">
         <v>0.865</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="7" t="n">
+        <v>0.787</v>
+      </c>
+      <c r="E16" s="7" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="F16" s="7" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="G16" s="7" t="n">
+        <v>0.7405</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>0.765</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
+      <c r="A17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="7" t="n">
+        <v>0.8635</v>
+      </c>
+      <c r="E17" s="7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="7" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="G17" s="7" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="I17" s="7" t="n">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+      <c r="B18" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="7" t="n">
+        <v>0.862</v>
+      </c>
+      <c r="E18" s="7" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="F18" s="7" t="n">
+        <v>0.895</v>
+      </c>
+      <c r="G18" s="7" t="n">
+        <v>0.8265</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>0.865</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
+      <c r="A19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="7" t="n">
+        <v>0.8265</v>
+      </c>
+      <c r="E19" s="7" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="F19" s="7" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="H19" s="7" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="I19" s="7" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="7" t="n">
+        <v>0.7975</v>
+      </c>
+      <c r="E20" s="7" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="F20" s="7" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="G20" s="7" t="n">
+        <v>0.7905</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="I20" s="7" t="n">
+        <v>0.825</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="7" t="n">
+        <v>0.801</v>
+      </c>
+      <c r="E21" s="7" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="F21" s="7" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="G21" s="7" t="n">
+        <v>0.7915</v>
+      </c>
+      <c r="H21" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I21" s="7" t="n">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+      <c r="A22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="7" t="n">
-        <v>0.787</v>
-      </c>
-      <c r="D16" s="7" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="E16" s="7" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="F16" s="7" t="n">
-        <v>0.7405</v>
-      </c>
-      <c r="G16" s="7" t="n">
-        <v>0.69</v>
-      </c>
-      <c r="H16" s="7" t="n">
-        <v>0.765</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
-      <c r="A19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="20">
-      <c r="A20" s="5" t="s">
+      <c r="B22" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="7" t="n">
+        <v>0.7785</v>
+      </c>
+      <c r="E22" s="7" t="n">
+        <v>0.705</v>
+      </c>
+      <c r="F22" s="7" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="G22" s="7" t="n">
+        <v>0.7615</v>
+      </c>
+      <c r="H22" s="7" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="I22" s="7" t="n">
+        <v>0.805</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="7" t="n">
+        <v>0.769</v>
+      </c>
+      <c r="E23" s="7" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="F23" s="7" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="G23" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H23" s="7" t="n">
+        <v>0.695</v>
+      </c>
+      <c r="I23" s="7" t="n">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="7" t="n">
+        <v>0.748</v>
+      </c>
+      <c r="E24" s="7" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F24" s="7" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="G24" s="7" t="n">
+        <v>0.743</v>
+      </c>
+      <c r="H24" s="7" t="n">
+        <v>0.695</v>
+      </c>
+      <c r="I24" s="7" t="n">
+        <v>0.785</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="A27" s="0"/>
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="A29" s="0"/>
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="31">
+      <c r="A31" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
-      <c r="A21" s="4" t="s">
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+      <c r="A32" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="H32" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="I32" s="6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="22">
-      <c r="A22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="7" t="n">
-        <v>0.8165</v>
-      </c>
-      <c r="D22" s="7" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="E22" s="7" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="F22" s="7" t="n">
-        <v>0.827</v>
-      </c>
-      <c r="G22" s="7" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="H22" s="7" t="n">
-        <v>0.865</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
-      <c r="B23" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="7" t="n">
-        <v>0.8195</v>
-      </c>
-      <c r="D23" s="7" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="E23" s="7" t="n">
-        <v>0.875</v>
-      </c>
-      <c r="F23" s="7" t="n">
-        <v>0.8245</v>
-      </c>
-      <c r="G23" s="7" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="H23" s="7" t="n">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
-      <c r="B24" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="C24" s="7" t="n">
-        <v>0.8215</v>
-      </c>
-      <c r="D24" s="7" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="E24" s="7" t="n">
-        <v>0.885</v>
-      </c>
-      <c r="F24" s="7" t="n">
-        <v>0.8215</v>
-      </c>
-      <c r="G24" s="7" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="H24" s="7" t="n">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
-      <c r="A25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="7" t="n">
-        <v>0.8115</v>
-      </c>
-      <c r="D25" s="7" t="n">
-        <v>0.735</v>
-      </c>
-      <c r="E25" s="7" t="n">
-        <v>0.855</v>
-      </c>
-      <c r="F25" s="7" t="n">
-        <v>0.818</v>
-      </c>
-      <c r="G25" s="7" t="n">
-        <v>0.785</v>
-      </c>
-      <c r="H25" s="7" t="n">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
-      <c r="B26" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="7" t="n">
-        <v>0.8035</v>
-      </c>
-      <c r="D26" s="7" t="n">
-        <v>0.755</v>
-      </c>
-      <c r="E26" s="7" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="F26" s="7" t="n">
-        <v>0.806</v>
-      </c>
-      <c r="G26" s="7" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="H26" s="7" t="n">
-        <v>0.845</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
-      <c r="B27" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C27" s="7" t="n">
-        <v>0.8105</v>
-      </c>
-      <c r="D27" s="7" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="E27" s="7" t="n">
-        <v>0.845</v>
-      </c>
-      <c r="F27" s="7" t="n">
-        <v>0.8005</v>
-      </c>
-      <c r="G27" s="7" t="n">
-        <v>0.745</v>
-      </c>
-      <c r="H27" s="7" t="n">
-        <v>0.845</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
-      <c r="B28" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="C28" s="7" t="n">
-        <v>0.8115</v>
-      </c>
-      <c r="D28" s="7" t="n">
-        <v>0.785</v>
-      </c>
-      <c r="E28" s="7" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="F28" s="7" t="n">
-        <v>0.7915</v>
-      </c>
-      <c r="G28" s="7" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="H28" s="7" t="n">
-        <v>0.835</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
-      <c r="A29" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="7" t="n">
-        <v>0.8095</v>
-      </c>
-      <c r="D29" s="7" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="E29" s="7" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="F29" s="7" t="n">
-        <v>0.8155</v>
-      </c>
-      <c r="G29" s="7" t="n">
-        <v>0.785</v>
-      </c>
-      <c r="H29" s="7" t="n">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
-      <c r="B30" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="7" t="n">
-        <v>0.7825</v>
-      </c>
-      <c r="D30" s="7" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="E30" s="7" t="n">
-        <v>0.815</v>
-      </c>
-      <c r="F30" s="7" t="n">
-        <v>0.789</v>
-      </c>
-      <c r="G30" s="7" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="H30" s="7" t="n">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
-      <c r="B31" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C31" s="7" t="n">
-        <v>0.7805</v>
-      </c>
-      <c r="D31" s="7" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="E31" s="7" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="F31" s="7" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="G31" s="7" t="n">
-        <v>0.735</v>
-      </c>
-      <c r="H31" s="7" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="B32" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C32" s="7" t="n">
-        <v>0.7665</v>
-      </c>
-      <c r="D32" s="7" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="E32" s="7" t="n">
-        <v>0.81</v>
-      </c>
-      <c r="F32" s="7" t="n">
-        <v>0.775</v>
-      </c>
-      <c r="G32" s="7" t="n">
-        <v>0.725</v>
-      </c>
-      <c r="H32" s="7" t="n">
-        <v>0.81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="33">
       <c r="A33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="7" t="n">
+        <v>0.8165</v>
+      </c>
+      <c r="E33" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F33" s="7" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="G33" s="7" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="H33" s="7" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="I33" s="7" t="n">
+        <v>0.865</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="B34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="7" t="n">
+        <v>0.8195</v>
+      </c>
+      <c r="E34" s="7" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="F34" s="7" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="G34" s="7" t="n">
+        <v>0.8245</v>
+      </c>
+      <c r="H34" s="7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I34" s="7" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="B35" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="7" t="n">
+        <v>0.8215</v>
+      </c>
+      <c r="E35" s="7" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="F35" s="7" t="n">
+        <v>0.885</v>
+      </c>
+      <c r="G35" s="7" t="n">
+        <v>0.8215</v>
+      </c>
+      <c r="H35" s="7" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="I35" s="7" t="n">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="36">
+      <c r="A36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="7" t="n">
+        <v>0.8115</v>
+      </c>
+      <c r="E36" s="7" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="F36" s="7" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="G36" s="7" t="n">
+        <v>0.818</v>
+      </c>
+      <c r="H36" s="7" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="I36" s="7" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+      <c r="B37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="7" t="n">
+        <v>0.8035</v>
+      </c>
+      <c r="E37" s="7" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="F37" s="7" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="G37" s="7" t="n">
+        <v>0.806</v>
+      </c>
+      <c r="H37" s="7" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="I37" s="7" t="n">
+        <v>0.845</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
+      <c r="B38" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="7" t="n">
+        <v>0.8105</v>
+      </c>
+      <c r="E38" s="7" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F38" s="7" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="G38" s="7" t="n">
+        <v>0.8005</v>
+      </c>
+      <c r="H38" s="7" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="I38" s="7" t="n">
+        <v>0.845</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
+      <c r="B39" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="7" t="n">
+        <v>0.8115</v>
+      </c>
+      <c r="E39" s="7" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="F39" s="7" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="G39" s="7" t="n">
+        <v>0.7915</v>
+      </c>
+      <c r="H39" s="7" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="I39" s="7" t="n">
+        <v>0.835</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+      <c r="A40" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="7" t="n">
+        <v>0.8095</v>
+      </c>
+      <c r="E40" s="7" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="F40" s="7" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="G40" s="7" t="n">
+        <v>0.8155</v>
+      </c>
+      <c r="H40" s="7" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="I40" s="7" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+      <c r="B41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="7" t="n">
+        <v>0.7825</v>
+      </c>
+      <c r="E41" s="7" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="F41" s="7" t="n">
+        <v>0.815</v>
+      </c>
+      <c r="G41" s="7" t="n">
+        <v>0.789</v>
+      </c>
+      <c r="H41" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I41" s="7" t="n">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+      <c r="B42" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="7" t="n">
+        <v>0.7805</v>
+      </c>
+      <c r="E42" s="7" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="F42" s="7" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="G42" s="7" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="H42" s="7" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="I42" s="7" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+      <c r="B43" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="7" t="n">
+        <v>0.7665</v>
+      </c>
+      <c r="E43" s="7" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="F43" s="7" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="G43" s="7" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="H43" s="7" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="I43" s="7" t="n">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="44">
+      <c r="A44" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="7" t="n">
+        <v>0.8145</v>
+      </c>
+      <c r="E44" s="7" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="F44" s="7" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="G44" s="7" t="n">
+        <v>0.8185</v>
+      </c>
+      <c r="H44" s="7" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="I44" s="7" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
+      <c r="A45" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="7" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="E45" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F45" s="7" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="G45" s="7" t="n">
+        <v>0.7515</v>
+      </c>
+      <c r="H45" s="7" t="n">
+        <v>0.685</v>
+      </c>
+      <c r="I45" s="7" t="n">
+        <v>0.825</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="46">
+      <c r="A46" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="7" t="n">
-        <v>0.8145</v>
-      </c>
-      <c r="D33" s="7" t="n">
+      <c r="B46" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="7" t="n">
+        <v>0.8245</v>
+      </c>
+      <c r="E46" s="7" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="F46" s="7" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="G46" s="7" t="n">
+        <v>0.818</v>
+      </c>
+      <c r="H46" s="7" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="I46" s="7" t="n">
+        <v>0.855</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
+      <c r="B47" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" s="7" t="n">
+        <v>0.8205</v>
+      </c>
+      <c r="E47" s="7" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="F47" s="7" t="n">
+        <v>0.865</v>
+      </c>
+      <c r="G47" s="7" t="n">
+        <v>0.8085</v>
+      </c>
+      <c r="H47" s="7" t="n">
         <v>0.745</v>
       </c>
-      <c r="E33" s="7" t="n">
-        <v>0.855</v>
-      </c>
-      <c r="F33" s="7" t="n">
-        <v>0.8185</v>
-      </c>
-      <c r="G33" s="7" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="H33" s="7" t="n">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
-      <c r="A34" s="3" t="s">
+      <c r="I47" s="7" t="n">
+        <v>0.845</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="48">
+      <c r="A48" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="7" t="n">
+        <v>0.8075</v>
+      </c>
+      <c r="E48" s="7" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="F48" s="7" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="G48" s="7" t="n">
+        <v>0.8045</v>
+      </c>
+      <c r="H48" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I48" s="7" t="n">
+        <v>0.835</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="7" t="n">
+        <v>0.8025</v>
+      </c>
+      <c r="E49" s="7" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F49" s="7" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="G49" s="7" t="n">
+        <v>0.794</v>
+      </c>
+      <c r="H49" s="7" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="I49" s="7" t="n">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" s="7" t="n">
+        <v>0.7985</v>
+      </c>
+      <c r="E50" s="7" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="F50" s="7" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="G50" s="7" t="n">
+        <v>0.784</v>
+      </c>
+      <c r="H50" s="7" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="I50" s="7" t="n">
+        <v>0.825</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
+      <c r="A51" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="7" t="n">
-        <v>0.785</v>
-      </c>
-      <c r="D34" s="7" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="E34" s="7" t="n">
-        <v>0.825</v>
-      </c>
-      <c r="F34" s="7" t="n">
-        <v>0.7515</v>
-      </c>
-      <c r="G34" s="7" t="n">
-        <v>0.685</v>
-      </c>
-      <c r="H34" s="7" t="n">
-        <v>0.825</v>
+      <c r="B51" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D51" s="7" t="n">
+        <v>0.7895</v>
+      </c>
+      <c r="E51" s="7" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="F51" s="7" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="G51" s="7" t="n">
+        <v>0.775</v>
+      </c>
+      <c r="H51" s="7" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="I51" s="7" t="n">
+        <v>0.815</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" s="7" t="n">
+        <v>0.773</v>
+      </c>
+      <c r="E52" s="7" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="F52" s="7" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="G52" s="7" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="H52" s="7" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="I52" s="7" t="n">
+        <v>0.795</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="7" t="n">
+        <v>0.757</v>
+      </c>
+      <c r="E53" s="7" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="F53" s="7" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="G53" s="7" t="n">
+        <v>0.753</v>
+      </c>
+      <c r="H53" s="7" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="I53" s="7" t="n">
+        <v>0.765</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:I31"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -6484,49 +7058,49 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>9</v>
@@ -7209,49 +7783,49 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="T17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="W17" s="2" t="s">
         <v>9</v>
@@ -8017,49 +8591,49 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>9</v>
@@ -8525,7 +9099,7 @@
       <c r="D12" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="8" t="n">
+      <c r="E12" s="9" t="n">
         <v>0.619048</v>
       </c>
       <c r="G12" s="0" t="s">
@@ -8742,49 +9316,49 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="T17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="W17" s="2" t="s">
         <v>9</v>
@@ -9480,17 +10054,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H41" activeCellId="0" pane="topLeft" sqref="H41"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G44" activeCellId="0" pane="topLeft" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="3" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -9504,22 +10078,26 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="I1" s="4"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="4" t="s">
@@ -9528,475 +10106,1061 @@
       <c r="B3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="J3" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="7" t="n">
         <v>0.6488095</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="E4" s="7" t="n">
         <v>0.583333</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="F4" s="7" t="n">
         <v>0.726191</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="G4" s="7" t="n">
         <v>0.6369048</v>
       </c>
-      <c r="G4" s="7" t="n">
+      <c r="H4" s="7" t="n">
         <v>0.535714</v>
       </c>
-      <c r="H4" s="7" t="n">
+      <c r="I4" s="7" t="n">
         <v>0.678571</v>
       </c>
+      <c r="J4" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="B5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="7" t="n">
         <v>0.6738096</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="E5" s="7" t="n">
         <v>0.607143</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="F5" s="7" t="n">
         <v>0.75</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="G5" s="7" t="n">
         <v>0.6190476</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="H5" s="7" t="n">
         <v>0.52381</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="I5" s="7" t="n">
         <v>0.702381</v>
       </c>
+      <c r="J5" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="7" t="n">
         <v>0.6547618</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="E6" s="7" t="n">
         <v>0.583333</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="F6" s="7" t="n">
         <v>0.738095</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="G6" s="7" t="n">
         <v>0.6095238</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="H6" s="7" t="n">
         <v>0.535714</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="I6" s="7" t="n">
         <v>0.654762</v>
       </c>
+      <c r="J6" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="B7" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="7" t="n">
         <v>0.6369048</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="E7" s="7" t="n">
         <v>0.559524</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="F7" s="7" t="n">
         <v>0.714286</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="G7" s="7" t="n">
         <v>0.6000001</v>
       </c>
-      <c r="G7" s="7" t="n">
+      <c r="H7" s="7" t="n">
         <v>0.559524</v>
       </c>
-      <c r="H7" s="7" t="n">
+      <c r="I7" s="7" t="n">
         <v>0.642857</v>
       </c>
+      <c r="J7" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="B8" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="7" t="n">
         <v>0.6142857</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="E8" s="7" t="n">
         <v>0.583333</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="F8" s="7" t="n">
         <v>0.690476</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="G8" s="7" t="n">
         <v>0.6107142</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="H8" s="7" t="n">
         <v>0.535714</v>
       </c>
-      <c r="H8" s="7" t="n">
+      <c r="I8" s="7" t="n">
         <v>0.690476</v>
       </c>
+      <c r="J8" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="7" t="n">
         <v>0.6019364</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="E9" s="7" t="n">
         <v>0.547619</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="F9" s="7" t="n">
         <v>0.678571</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="G9" s="7" t="n">
         <v>0.5641136</v>
       </c>
-      <c r="G9" s="7" t="n">
+      <c r="H9" s="7" t="n">
         <v>0.457831</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="I9" s="7" t="n">
         <v>0.626506</v>
       </c>
+      <c r="J9" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="B10" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="7" t="n">
         <v>0.5313931</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="E10" s="7" t="n">
         <v>0.404762</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="F10" s="7" t="n">
         <v>0.583333</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="G10" s="7" t="n">
         <v>0.5377798</v>
       </c>
-      <c r="G10" s="7" t="n">
+      <c r="H10" s="7" t="n">
         <v>0.493976</v>
       </c>
-      <c r="H10" s="7" t="n">
+      <c r="I10" s="7" t="n">
         <v>0.590362</v>
       </c>
+      <c r="J10" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="B11" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="7" t="n">
         <v>0.5565836</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="E11" s="7" t="n">
         <v>0.511905</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="F11" s="7" t="n">
         <v>0.607143</v>
       </c>
-      <c r="F11" s="7" t="n">
+      <c r="G11" s="7" t="n">
         <v>0.5556512</v>
       </c>
-      <c r="G11" s="7" t="n">
+      <c r="H11" s="7" t="n">
         <v>0.476191</v>
       </c>
-      <c r="H11" s="7" t="n">
+      <c r="I11" s="7" t="n">
         <v>0.630952</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="A14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
-      <c r="A15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4" t="s">
+      <c r="J11" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
+      <c r="A12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="D12" s="7" t="n">
+        <v>0.651191</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="F12" s="7" t="n">
+        <v>0.714286</v>
+      </c>
+      <c r="G12" s="7" t="n">
+        <v>0.629762</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="B13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <v>0.6392857</v>
+      </c>
+      <c r="E13" s="7" t="n">
+        <v>0.5238095</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <v>0.714286</v>
+      </c>
+      <c r="G13" s="7" t="n">
+        <v>0.61666667</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>0.511905</v>
+      </c>
+      <c r="I13" s="7" t="n">
+        <v>0.738095</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
+      <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <v>0.652381</v>
+      </c>
+      <c r="E14" s="7" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="F14" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G14" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="I14" s="7" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="B15" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <v>0.617857</v>
+      </c>
+      <c r="E15" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <v>0.66666666</v>
+      </c>
+      <c r="G15" s="7" t="n">
+        <v>0.609524</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="I15" s="7" t="n">
+        <v>0.66666667</v>
+      </c>
+      <c r="J15" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
-      <c r="A16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
+      <c r="B16" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="7" t="n">
+        <v>0.580952</v>
+      </c>
+      <c r="E16" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="F16" s="7" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="G16" s="7" t="n">
+        <v>0.620238</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>0.71429</v>
+      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="7" t="n">
-        <v>0.6738096</v>
+      <c r="C17" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D17" s="7" t="n">
-        <v>0.607143</v>
+        <v>0.603141</v>
       </c>
       <c r="E17" s="7" t="n">
-        <v>0.75</v>
+        <v>0.547619</v>
       </c>
       <c r="F17" s="7" t="n">
-        <v>0.6452381</v>
+        <v>0.690476</v>
       </c>
       <c r="G17" s="7" t="n">
-        <v>0.583333</v>
+        <v>0.566495</v>
       </c>
       <c r="H17" s="7" t="n">
-        <v>0.714286</v>
-      </c>
+        <v>0.457831</v>
+      </c>
+      <c r="I17" s="7" t="n">
+        <v>0.626506</v>
+      </c>
+      <c r="J17" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="B18" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="7" t="n">
+        <v>0.550617</v>
+      </c>
+      <c r="E18" s="7" t="n">
+        <v>0.452381</v>
+      </c>
+      <c r="F18" s="7" t="n">
+        <v>0.67857</v>
+      </c>
+      <c r="G18" s="7" t="n">
+        <v>0.540146</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <v>0.488095</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>0.5903615</v>
+      </c>
+      <c r="J18" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+      <c r="B19" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="7" t="n">
+        <v>0.5553499</v>
+      </c>
+      <c r="E19" s="7" t="n">
+        <v>0.4939759</v>
+      </c>
+      <c r="F19" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>0.556856</v>
+      </c>
+      <c r="H19" s="7" t="n">
+        <v>0.47619</v>
+      </c>
+      <c r="I19" s="7" t="n">
+        <v>0.61905</v>
+      </c>
+      <c r="J19" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+      <c r="A25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="A26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+      <c r="A27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="28">
+      <c r="A28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="7" t="n">
+        <v>0.6738096</v>
+      </c>
+      <c r="E28" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="F28" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G28" s="7" t="n">
+        <v>0.6452381</v>
+      </c>
+      <c r="H28" s="7" t="n">
+        <v>0.583333</v>
+      </c>
+      <c r="I28" s="7" t="n">
+        <v>0.714286</v>
+      </c>
+      <c r="J28" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+      <c r="B29" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="7" t="n">
         <v>0.6202381</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="E29" s="7" t="n">
         <v>0.571429</v>
       </c>
-      <c r="E18" s="7" t="n">
+      <c r="F29" s="7" t="n">
         <v>0.702381</v>
       </c>
-      <c r="F18" s="7" t="n">
+      <c r="G29" s="7" t="n">
         <v>0.6559523</v>
       </c>
-      <c r="G18" s="7" t="n">
+      <c r="H29" s="7" t="n">
         <v>0.583333</v>
       </c>
-      <c r="H18" s="7" t="n">
+      <c r="I29" s="7" t="n">
         <v>0.785714</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
-      <c r="A19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="3" t="n">
+      <c r="J29" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="30">
+      <c r="A30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C19" s="7" t="n">
+      <c r="C30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="7" t="n">
         <v>0.6833334</v>
       </c>
-      <c r="D19" s="7" t="n">
+      <c r="E30" s="7" t="n">
         <v>0.595238</v>
       </c>
-      <c r="E19" s="7" t="n">
+      <c r="F30" s="7" t="n">
         <v>0.77381</v>
       </c>
-      <c r="F19" s="7" t="n">
+      <c r="G30" s="7" t="n">
         <v>0.6380951</v>
       </c>
-      <c r="G19" s="7" t="n">
+      <c r="H30" s="7" t="n">
         <v>0.535714</v>
       </c>
-      <c r="H19" s="7" t="n">
+      <c r="I30" s="7" t="n">
         <v>0.726191</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
-      <c r="B20" s="3" t="n">
+      <c r="J30" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+      <c r="B31" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="C31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="7" t="n">
         <v>0.5952379</v>
       </c>
-      <c r="D20" s="7" t="n">
+      <c r="E31" s="7" t="n">
         <v>0.535714</v>
       </c>
-      <c r="E20" s="7" t="n">
+      <c r="F31" s="7" t="n">
         <v>0.654762</v>
       </c>
-      <c r="F20" s="7" t="n">
+      <c r="G31" s="7" t="n">
         <v>0.6214286</v>
       </c>
-      <c r="G20" s="7" t="n">
+      <c r="H31" s="7" t="n">
         <v>0.52381</v>
       </c>
-      <c r="H20" s="7" t="n">
+      <c r="I31" s="7" t="n">
         <v>0.726191</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
-      <c r="B21" s="3" t="n">
+      <c r="J31" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+      <c r="B32" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="7" t="n">
         <v>0.6130953</v>
       </c>
-      <c r="D21" s="7" t="n">
+      <c r="E32" s="7" t="n">
         <v>0.535714</v>
       </c>
-      <c r="E21" s="7" t="n">
+      <c r="F32" s="7" t="n">
         <v>0.666667</v>
       </c>
-      <c r="F21" s="7" t="n">
+      <c r="G32" s="7" t="n">
         <v>0.6071426</v>
       </c>
-      <c r="G21" s="7" t="n">
+      <c r="H32" s="7" t="n">
         <v>0.535714</v>
       </c>
-      <c r="H21" s="7" t="n">
+      <c r="I32" s="7" t="n">
         <v>0.690476</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
-      <c r="A22" s="3" t="s">
+      <c r="J32" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+      <c r="A33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="D33" s="7" t="n">
+        <v>0.6174411</v>
+      </c>
+      <c r="E33" s="7" t="n">
+        <v>0.535714</v>
+      </c>
+      <c r="F33" s="7" t="n">
+        <v>0.702381</v>
+      </c>
+      <c r="G33" s="7" t="n">
+        <v>0.5999713</v>
+      </c>
+      <c r="H33" s="7" t="n">
+        <v>0.476191</v>
+      </c>
+      <c r="I33" s="7" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="J33" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="B34" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="7" t="n">
+        <v>0.5565692</v>
+      </c>
+      <c r="E34" s="7" t="n">
+        <v>0.464286</v>
+      </c>
+      <c r="F34" s="7" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="G34" s="7" t="n">
+        <v>0.499326</v>
+      </c>
+      <c r="H34" s="7" t="n">
+        <v>0.433735</v>
+      </c>
+      <c r="I34" s="7" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="J34" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="B35" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="7" t="n">
+        <v>0.5590219</v>
+      </c>
+      <c r="E35" s="7" t="n">
+        <v>0.511905</v>
+      </c>
+      <c r="F35" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="G35" s="7" t="n">
+        <v>0.5137694</v>
+      </c>
+      <c r="H35" s="7" t="n">
+        <v>0.428571</v>
+      </c>
+      <c r="I35" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="J35" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="36">
+      <c r="A36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C22" s="7" t="n">
-        <v>0.6174411</v>
-      </c>
-      <c r="D22" s="7" t="n">
-        <v>0.535714</v>
-      </c>
-      <c r="E22" s="7" t="n">
+      <c r="C36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="7" t="n">
+        <v>0.665476</v>
+      </c>
+      <c r="E36" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="F36" s="7" t="n">
+        <v>0.7261905</v>
+      </c>
+      <c r="G36" s="7" t="n">
+        <v>0.642857</v>
+      </c>
+      <c r="H36" s="7" t="n">
+        <v>0.559524</v>
+      </c>
+      <c r="I36" s="7" t="n">
+        <v>0.72619</v>
+      </c>
+      <c r="J36" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+      <c r="B37" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="7" t="n">
+        <v>0.6345238</v>
+      </c>
+      <c r="E37" s="7" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="F37" s="7" t="n">
+        <v>0.738095</v>
+      </c>
+      <c r="G37" s="7" t="n">
+        <v>0.660714</v>
+      </c>
+      <c r="H37" s="7" t="n">
+        <v>0.5833333</v>
+      </c>
+      <c r="I37" s="7" t="n">
+        <v>0.785714</v>
+      </c>
+      <c r="J37" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="38">
+      <c r="A38" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="7" t="n">
+        <v>0.67619</v>
+      </c>
+      <c r="E38" s="7" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="F38" s="7" t="n">
+        <v>0.738095</v>
+      </c>
+      <c r="G38" s="7" t="n">
+        <v>0.632143</v>
+      </c>
+      <c r="H38" s="7" t="n">
+        <v>0.52381</v>
+      </c>
+      <c r="I38" s="7" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J38" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
+      <c r="B39" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="7" t="n">
+        <v>0.595238</v>
+      </c>
+      <c r="E39" s="7" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="F39" s="7" t="n">
+        <v>0.678571</v>
+      </c>
+      <c r="G39" s="7" t="n">
+        <v>0.61666667</v>
+      </c>
+      <c r="H39" s="7" t="n">
+        <v>0.5238095</v>
+      </c>
+      <c r="I39" s="7" t="n">
+        <v>0.7261905</v>
+      </c>
+      <c r="J39" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+      <c r="B40" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="7" t="n">
+        <v>0.580952</v>
+      </c>
+      <c r="E40" s="7" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="F40" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="G40" s="7" t="n">
+        <v>0.607143</v>
+      </c>
+      <c r="H40" s="7" t="n">
+        <v>0.511905</v>
+      </c>
+      <c r="I40" s="7" t="n">
+        <v>0.690476</v>
+      </c>
+      <c r="J40" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+      <c r="A41" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="7" t="n">
+        <v>0.618632</v>
+      </c>
+      <c r="E41" s="7" t="n">
+        <v>0.5357143</v>
+      </c>
+      <c r="F41" s="7" t="n">
         <v>0.702381</v>
       </c>
-      <c r="F22" s="7" t="n">
-        <v>0.5999713</v>
-      </c>
-      <c r="G22" s="7" t="n">
-        <v>0.476191</v>
-      </c>
-      <c r="H22" s="7" t="n">
-        <v>0.678571</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
-      <c r="B23" s="3" t="n">
+      <c r="G41" s="7" t="n">
+        <v>0.6023666</v>
+      </c>
+      <c r="H41" s="7" t="n">
+        <v>0.488095</v>
+      </c>
+      <c r="I41" s="7" t="n">
+        <v>0.67857</v>
+      </c>
+      <c r="J41" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+      <c r="B42" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C23" s="7" t="n">
-        <v>0.5565692</v>
-      </c>
-      <c r="D23" s="7" t="n">
-        <v>0.464286</v>
-      </c>
-      <c r="E23" s="7" t="n">
+      <c r="C42" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="7" t="n">
+        <v>0.548164</v>
+      </c>
+      <c r="E42" s="7" t="n">
+        <v>0.452381</v>
+      </c>
+      <c r="F42" s="7" t="n">
         <v>0.642857</v>
       </c>
-      <c r="F23" s="7" t="n">
-        <v>0.499326</v>
-      </c>
-      <c r="G23" s="7" t="n">
-        <v>0.433735</v>
-      </c>
-      <c r="H23" s="7" t="n">
-        <v>0.559524</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
-      <c r="B24" s="3" t="n">
+      <c r="G42" s="7" t="n">
+        <v>0.496959</v>
+      </c>
+      <c r="H42" s="7" t="n">
+        <v>0.445783</v>
+      </c>
+      <c r="I42" s="7" t="n">
+        <v>0.547619</v>
+      </c>
+      <c r="J42" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+      <c r="B43" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C24" s="7" t="n">
-        <v>0.5590219</v>
-      </c>
-      <c r="D24" s="7" t="n">
+      <c r="C43" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="7" t="n">
+        <v>0.5578313</v>
+      </c>
+      <c r="E43" s="7" t="n">
         <v>0.511905</v>
       </c>
-      <c r="E24" s="7" t="n">
+      <c r="F43" s="7" t="n">
         <v>0.607143</v>
       </c>
-      <c r="F24" s="7" t="n">
-        <v>0.5137694</v>
-      </c>
-      <c r="G24" s="7" t="n">
-        <v>0.428571</v>
-      </c>
-      <c r="H24" s="7" t="n">
-        <v>0.607143</v>
-      </c>
+      <c r="G43" s="7" t="n">
+        <v>0.506612</v>
+      </c>
+      <c r="H43" s="7" t="n">
+        <v>0.44047619</v>
+      </c>
+      <c r="I43" s="7" t="n">
+        <v>0.58333333</v>
+      </c>
+      <c r="J43" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A25:I25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add results for using sentiment lexicon features with negation tagged text.
</commit_message>
<xml_diff>
--- a/results_summary.xlsx
+++ b/results_summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="48">
   <si>
     <t>features:</t>
   </si>
@@ -5652,10 +5652,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H39" activeCellId="0" pane="topLeft" sqref="H39"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G50" activeCellId="0" pane="topLeft" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6299,15 +6299,33 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
-      <c r="A25" s="0"/>
-      <c r="B25" s="0"/>
-      <c r="C25" s="0"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="A25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="7" t="n">
+        <v>0.7825</v>
+      </c>
+      <c r="E25" s="7" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="F25" s="7" t="n">
+        <v>0.845</v>
+      </c>
+      <c r="G25" s="7" t="n">
+        <v>0.731</v>
+      </c>
+      <c r="H25" s="7" t="n">
+        <v>0.685</v>
+      </c>
+      <c r="I25" s="7" t="n">
+        <v>0.78</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0"/>
@@ -6960,6 +6978,35 @@
       </c>
       <c r="I53" s="7" t="n">
         <v>0.765</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
+      <c r="A54" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54" s="7" t="n">
+        <v>0.789</v>
+      </c>
+      <c r="E54" s="7" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="F54" s="7" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="G54" s="7" t="n">
+        <v>0.7525</v>
+      </c>
+      <c r="H54" s="7" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I54" s="7" t="n">
+        <v>0.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>